<commit_message>
completed regional var worksheet
</commit_message>
<xml_diff>
--- a/CSV_TO_JSON/tmp/regional v02_variables.xlsx
+++ b/CSV_TO_JSON/tmp/regional v02_variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="424">
   <si>
     <t>srce + target</t>
   </si>
@@ -1214,6 +1214,84 @@
   </si>
   <si>
     <t>RUCCYHF, RUCCYHH</t>
+  </si>
+  <si>
+    <t>RUFXBRR</t>
+  </si>
+  <si>
+    <t>RUFXBRF, RUFXBRZ, RUFXBRH</t>
+  </si>
+  <si>
+    <t>RUFXTRF</t>
+  </si>
+  <si>
+    <t>RUINTRF, RUINTRH</t>
+  </si>
+  <si>
+    <t>RUPARMF, RUPARMH</t>
+  </si>
+  <si>
+    <t>RUPARRF</t>
+  </si>
+  <si>
+    <t>RUTRLOGR</t>
+  </si>
+  <si>
+    <t>RUR002P, RUR003P, RUR009P, RUR012P, RUR013P</t>
+  </si>
+  <si>
+    <t>RUSROBR</t>
+  </si>
+  <si>
+    <t>RUSROSP</t>
+  </si>
+  <si>
+    <t>RUAV</t>
+  </si>
+  <si>
+    <t>RUFU</t>
+  </si>
+  <si>
+    <t>RUSG</t>
+  </si>
+  <si>
+    <t>RUSROBUF</t>
+  </si>
+  <si>
+    <t>RUBU</t>
+  </si>
+  <si>
+    <t>RUSROHIE</t>
+  </si>
+  <si>
+    <t>RUSROSW</t>
+  </si>
+  <si>
+    <t>RUFXTRR</t>
+  </si>
+  <si>
+    <t>RUBUFFR</t>
+  </si>
+  <si>
+    <t>RUSPFXF, RUSPFXZ</t>
+  </si>
+  <si>
+    <t>RUSPGLF, RUSPGLH</t>
+  </si>
+  <si>
+    <t>RUSPOTF, RUSPOTH</t>
+  </si>
+  <si>
+    <t>RUSWAPF, RUSWAPH</t>
+  </si>
+  <si>
+    <t>RUSWGLF, RUSWGLH</t>
+  </si>
+  <si>
+    <t>RUTENRF, RUTENRH</t>
+  </si>
+  <si>
+    <t>RUTRLOG</t>
   </si>
 </sst>
 </file>
@@ -2110,8 +2188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C314"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A230" workbookViewId="0">
-      <selection activeCell="C265" sqref="C265"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C312" sqref="C312"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4187,7 +4265,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" s="3" t="s">
         <v>244</v>
       </c>
@@ -4195,347 +4273,491 @@
         <v>391</v>
       </c>
     </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="B258" s="2"/>
-    </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B258" s="2" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A259" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="B259" s="2"/>
-    </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B259" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="C259" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="B260" s="2"/>
-    </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B260" s="2" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="B261" s="2"/>
-    </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B261" s="2" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="B262" s="2"/>
-    </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B262" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="C262" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="B263" s="2"/>
-    </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B263" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="C263" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="B264" s="2"/>
-    </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B264" s="2" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="B265" s="2"/>
-    </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B265" s="2" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="B266" s="2"/>
-    </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B266" s="2" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A267" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="B267" s="2"/>
-    </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B267" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C267" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="B268" s="2"/>
-    </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B268" s="2" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="B269" s="2"/>
-    </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B269" s="2" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="B270" s="2"/>
-    </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B270" s="2" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="B271" s="2"/>
-    </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B271" s="2" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="B272" s="2"/>
+      <c r="B272" s="2" t="s">
+        <v>408</v>
+      </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="B273" s="2"/>
+      <c r="B273" s="2" t="s">
+        <v>409</v>
+      </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="B274" s="2"/>
+      <c r="B274" s="2" t="s">
+        <v>410</v>
+      </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="B275" s="2"/>
+      <c r="B275" s="2" t="s">
+        <v>411</v>
+      </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="B276" s="2"/>
+      <c r="B276" s="2" t="s">
+        <v>404</v>
+      </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="B277" s="2"/>
+      <c r="B277" s="2" t="s">
+        <v>412</v>
+      </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="B278" s="2"/>
+      <c r="B278" s="2" t="s">
+        <v>413</v>
+      </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="B279" s="2"/>
+      <c r="B279" s="2" t="s">
+        <v>404</v>
+      </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="B280" s="2"/>
+      <c r="B280" s="2" t="s">
+        <v>406</v>
+      </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="B281" s="2"/>
+      <c r="B281" s="2" t="s">
+        <v>407</v>
+      </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A282" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="B282" s="2"/>
+      <c r="B282" s="2" t="s">
+        <v>404</v>
+      </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="B283" s="2"/>
+      <c r="B283" s="2" t="s">
+        <v>414</v>
+      </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A284" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="B284" s="2"/>
+      <c r="B284" s="2" t="s">
+        <v>404</v>
+      </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="B285" s="2"/>
+      <c r="B285" s="2" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A286" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="B286" s="2"/>
+      <c r="B286" s="2" t="s">
+        <v>398</v>
+      </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A287" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="B287" s="2"/>
+      <c r="B287" s="2" t="s">
+        <v>415</v>
+      </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A288" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="B288" s="2"/>
-    </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B288" s="2" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A289" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="B289" s="2"/>
-    </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B289" s="2" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A290" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="B290" s="2"/>
-    </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B290" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="C290" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A291" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="B291" s="2"/>
-    </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B291" s="2" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A292" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="B292" s="2"/>
-    </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B292" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="C292" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A293" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="B293" s="2"/>
-    </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B293" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="C293" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A294" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="B294" s="2"/>
-    </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B294" s="2" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A295" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="B295" s="2"/>
-    </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B295" s="2" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A296" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="B296" s="2"/>
-    </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B296" s="2" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A297" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="B297" s="2"/>
-    </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B297" s="2" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A298" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="B298" s="2"/>
-    </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B298" s="2" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A299" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="B299" s="2"/>
-    </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B299" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A300" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="B300" s="2"/>
-    </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B300" s="2" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A301" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="B301" s="2"/>
-    </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B301" s="2" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A302" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="B302" s="2"/>
-    </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B302" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A303" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="B303" s="2"/>
-    </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B303" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A304" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="B304" s="2"/>
-    </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B304" s="2" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A305" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="B305" s="2"/>
-    </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B305" s="2" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A306" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="B306" s="2"/>
-    </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B306" s="2" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A307" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="B307" s="2"/>
-    </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B307" s="2" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A308" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="B308" s="2"/>
-    </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B308" s="2" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A309" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="B309" s="2"/>
-    </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B309" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="C309" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A310" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="B310" s="2"/>
-    </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B310" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="C310" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A311" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="B311" s="2"/>
-    </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B311" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="C311" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A312" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="B312" s="2"/>
-    </row>
-    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B312" s="2" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A313" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="B313" s="2"/>
-    </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B313" s="2" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A314" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="B314" s="2"/>
+      <c r="B314" s="2" t="s">
+        <v>388</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>